<commit_message>
- created new test and test data for testing context-entries-generator - new test data for business model - some partial implementation for stuff in the decision-table tests
</commit_message>
<xml_diff>
--- a/test/data/PostBureauRiskCategory2.xlsx
+++ b/test/data/PostBureauRiskCategory2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Post-Bureau Risk Category Table" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Existing Customer</t>
   </si>
   <si>
-    <t>Post-Bureau Risk Category</t>
-  </si>
-  <si>
-    <t>Applicant . ExistingCustomer</t>
-  </si>
-  <si>
     <t>Credit Score</t>
   </si>
   <si>
@@ -90,16 +84,16 @@
     <t>&gt;600</t>
   </si>
   <si>
-    <t>Affordability Model(Applicant, Product) . Application Risk Score</t>
-  </si>
-  <si>
-    <t>Post-Bureau Risk Category Table</t>
-  </si>
-  <si>
     <t>Applicant. ExistingCustomer</t>
   </si>
   <si>
     <t>Affordability Model(Applicant, Product). Application Risk Score</t>
+  </si>
+  <si>
+    <t>Post Bureau Risk Category</t>
+  </si>
+  <si>
+    <t>Post Bureau Risk Category Table</t>
   </si>
 </sst>
 </file>
@@ -129,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -165,11 +159,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -183,6 +186,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,13 +470,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -491,23 +496,23 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -515,36 +520,36 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -555,13 +560,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -571,10 +576,10 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -584,10 +589,10 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -598,13 +603,13 @@
         <v>0</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -614,10 +619,10 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -627,10 +632,10 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -646,60 +651,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C8"/>
+  <dimension ref="A2:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
     <col min="3" max="3" width="41.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revising makeContext() related tests according to the new object it returns
</commit_message>
<xml_diff>
--- a/test/data/PostBureauRiskCategory2.xlsx
+++ b/test/data/PostBureauRiskCategory2.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Post-Bureau Risk Category Table" sheetId="1" r:id="rId1"/>
-    <sheet name="Post-Bureau Risk Category" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -123,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -159,20 +159,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -186,8 +177,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,35 +640,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C8"/>
+  <dimension ref="B2:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
@@ -687,7 +673,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -695,17 +681,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>